<commit_message>
mise en place des balises semantique dans les partie html
</commit_message>
<xml_diff>
--- a/audit seo et acces p4.xlsx
+++ b/audit seo et acces p4.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="87">
   <si>
     <t xml:space="preserve">Catégorie</t>
   </si>
@@ -253,19 +253,34 @@
     <t xml:space="preserve">https://seranking.com/fr/blog/comprendre-css-et-javascript-en-seo/</t>
   </si>
   <si>
-    <t xml:space="preserve">Il n’y as pas de balise meta</t>
+    <t xml:space="preserve">Il n’y as pas de balise meta Robots.</t>
   </si>
   <si>
     <t xml:space="preserve">Sans balise robots le referencement,seras moindre.La balise sert as indiquer si une pages peut etre indexer ou pas .</t>
   </si>
   <si>
-    <t xml:space="preserve">Mettre le codeci-dessous  dans le html &lt;metaname= ‘’robots’’ content= ‘’index’’&gt;</t>
+    <t xml:space="preserve">Mettre le code ci-dessous  dans le HTML &lt;meta name= ‘’robots’’ content= ‘’index’’&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">Inserer le code dans le html</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.webrankinfo.com/dossiers/conseils/balise-meta-robots?fbclid=IwAR0Ut1xFHbcIfJlyIxz2wMGeF0DgYY6e0_RBigwIw-2Q9-PrX7wha9mVRmc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">il n’yas pas de sitemap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sans le site map le site se seras entierement referencer </t>
+  </si>
+  <si>
+    <t xml:space="preserve">mettre une sitemap xml</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inserer le site map dans le code html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.sitemaps.org/protocol.html#location</t>
   </si>
 </sst>
 </file>
@@ -343,7 +358,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -354,6 +369,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF7030A0"/>
         <bgColor rgb="FF993366"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF2CEE0E"/>
+        <bgColor rgb="FF99CC00"/>
       </patternFill>
     </fill>
   </fills>
@@ -391,7 +412,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -432,11 +453,31 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -454,7 +495,7 @@
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
       <rgbColor rgb="FFFF0000"/>
-      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF2CEE0E"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
@@ -639,19 +680,19 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="65.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="12" t="s">
         <v>25</v>
       </c>
       <c r="F6" s="5" t="s">
@@ -659,19 +700,19 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="62.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="12" t="s">
         <v>30</v>
       </c>
       <c r="F7" s="5" t="s">
@@ -679,19 +720,19 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="63.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="12" t="s">
         <v>35</v>
       </c>
       <c r="F8" s="8" t="s">
@@ -699,19 +740,19 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="80.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="12" t="s">
         <v>39</v>
       </c>
       <c r="F9" s="5" t="s">
@@ -719,19 +760,19 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="12" t="s">
         <v>44</v>
       </c>
       <c r="F10" s="8" t="s">
@@ -751,7 +792,7 @@
       <c r="D11" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E11" s="13" t="s">
         <v>50</v>
       </c>
       <c r="F11" s="5" t="s">
@@ -759,19 +800,19 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="129.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="E12" s="15" t="s">
         <v>55</v>
       </c>
       <c r="F12" s="5" t="s">
@@ -779,19 +820,19 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="E13" s="16" t="s">
         <v>60</v>
       </c>
       <c r="F13" s="8" t="s">
@@ -799,19 +840,19 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="96.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="E14" s="15" t="s">
         <v>65</v>
       </c>
       <c r="F14" s="8" t="s">
@@ -819,19 +860,19 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="93.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="E15" s="15" t="s">
         <v>70</v>
       </c>
       <c r="F15" s="8" t="s">
@@ -878,7 +919,26 @@
         <v>81</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="18" customFormat="false" ht="93.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>86</v>
+      </c>
+    </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>